<commit_message>
new survey from UUE
</commit_message>
<xml_diff>
--- a/survey_resources/uue/uue-survey.xlsx
+++ b/survey_resources/uue/uue-survey.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="240">
   <si>
     <t>type</t>
   </si>
@@ -66,6 +66,18 @@
     <t>. = ${uniqueid}</t>
   </si>
   <si>
+    <t>study_phone_id</t>
+  </si>
+  <si>
+    <t>Study Phone ID</t>
+  </si>
+  <si>
+    <t>use 999 for respondent personal phone</t>
+  </si>
+  <si>
+    <t>string-length(.) = 3</t>
+  </si>
+  <si>
     <t>begin_group</t>
   </si>
   <si>
@@ -129,6 +141,9 @@
     <t>list_name</t>
   </si>
   <si>
+    <t>order</t>
+  </si>
+  <si>
     <t>zp4by70</t>
   </si>
   <si>
@@ -237,21 +252,300 @@
     <t>Other</t>
   </si>
   <si>
+    <t>eq7av60</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>hw6ou02</t>
+  </si>
+  <si>
+    <t>black_or_african_american</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>white_or_caucasian</t>
+  </si>
+  <si>
+    <t>White or Caucasian</t>
+  </si>
+  <si>
+    <t>hispanic_latino_a_x_or_spanish</t>
+  </si>
+  <si>
+    <t>Hispanic, Latino/a/x, or Spanish</t>
+  </si>
+  <si>
+    <t>east_asian</t>
+  </si>
+  <si>
+    <t>East Asian</t>
+  </si>
+  <si>
+    <t>south_asian</t>
+  </si>
+  <si>
+    <t>South Asian</t>
+  </si>
+  <si>
+    <t>american_indian_or_alaska_native</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>native_hawaiian_or_other_pacific_islande</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>multiracial_multiethnic</t>
+  </si>
+  <si>
+    <t>Multiracial/Multiethnic</t>
+  </si>
+  <si>
+    <t>mw0ph17</t>
+  </si>
+  <si>
+    <t>pz1ou68</t>
+  </si>
+  <si>
+    <t>not_a_student</t>
+  </si>
+  <si>
+    <t>Not A Student</t>
+  </si>
+  <si>
+    <t>yes___k_12th_grade_including_ged</t>
+  </si>
+  <si>
+    <t>Yes - K-12th Grade including GED</t>
+  </si>
+  <si>
+    <t>yes___vocation_technical_trade_school</t>
+  </si>
+  <si>
+    <t>Yes - Vocation/Technical/Trade School</t>
+  </si>
+  <si>
+    <t>yes___part_time_college_university</t>
+  </si>
+  <si>
+    <t>Yes - Part-Time college/University</t>
+  </si>
+  <si>
+    <t>yes___full_time_college_university</t>
+  </si>
+  <si>
+    <t>Yes - Full Time college/University</t>
+  </si>
+  <si>
+    <t>is7jb99</t>
+  </si>
+  <si>
+    <t>less_than_a_high_school_graduate</t>
+  </si>
+  <si>
+    <t>Less than a high school graduate</t>
+  </si>
+  <si>
+    <t>high_school_graduate_or_ged</t>
+  </si>
+  <si>
+    <t>High school graduate or GED</t>
+  </si>
+  <si>
+    <t>some_college_or_associates_degree</t>
+  </si>
+  <si>
+    <t>Some college or associates degree</t>
+  </si>
+  <si>
+    <t>bachelor_s_degree</t>
+  </si>
+  <si>
+    <t>Bachelor's degree</t>
+  </si>
+  <si>
+    <t>graduate_degree_or_professional_degree</t>
+  </si>
+  <si>
+    <t>Graduate degree or professional degree</t>
+  </si>
+  <si>
+    <t>bl0bx01</t>
+  </si>
+  <si>
+    <t>jk8cx93</t>
+  </si>
+  <si>
+    <t>i_m_temporarily_absent_from_a_job_now</t>
+  </si>
+  <si>
+    <t>I'm temporarily absent from a job now</t>
+  </si>
+  <si>
+    <t>i_m_not_able_to_work__due_to_reasons_lik</t>
+  </si>
+  <si>
+    <t>I'm not able to work (due to reasons like age, physical capability, etc.)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>none_of_the_above</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>mu0is58</t>
+  </si>
+  <si>
+    <t>own</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>neither</t>
+  </si>
+  <si>
+    <t>Neither</t>
+  </si>
+  <si>
+    <t>vm7wa34</t>
+  </si>
+  <si>
+    <t>condominium_apartment</t>
+  </si>
+  <si>
+    <t>Condominium/Apartment</t>
+  </si>
+  <si>
+    <t>single_family_house</t>
+  </si>
+  <si>
+    <t>Single Family House</t>
+  </si>
+  <si>
+    <t>multi_family_house</t>
+  </si>
+  <si>
+    <t>Multi-Family House</t>
+  </si>
+  <si>
+    <t>shelter</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>wc3ba24</t>
+  </si>
+  <si>
+    <t>less_than__24_999</t>
+  </si>
+  <si>
+    <t>Less than $24,999</t>
+  </si>
+  <si>
+    <t>_25_000_to__49_999</t>
+  </si>
+  <si>
+    <t>$25,000 to $49,999</t>
+  </si>
+  <si>
+    <t>_50_000_to__99_999</t>
+  </si>
+  <si>
+    <t>$50,000 to $99,999</t>
+  </si>
+  <si>
+    <t>_100_000_to__149_999</t>
+  </si>
+  <si>
+    <t>$100,000 to $149,999</t>
+  </si>
+  <si>
+    <t>_150_000_to__199_999</t>
+  </si>
+  <si>
+    <t>$150,000 to $199,999</t>
+  </si>
+  <si>
+    <t>_200_000_or_more</t>
+  </si>
+  <si>
+    <t>$200,000 or more</t>
+  </si>
+  <si>
+    <t>sk0vf59</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>more_than_7</t>
+  </si>
+  <si>
+    <t>More than 7</t>
+  </si>
+  <si>
+    <t>mb1ko67</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>more_than_4</t>
+  </si>
+  <si>
+    <t>More than 4</t>
+  </si>
+  <si>
+    <t>kt8vu83</t>
+  </si>
+  <si>
     <t>uf9mf06</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>more_than_3</t>
   </si>
   <si>
@@ -301,6 +595,129 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>zd44g49</t>
+  </si>
+  <si>
+    <t>gx7yn58</t>
+  </si>
+  <si>
+    <t>6_months_or_less</t>
+  </si>
+  <si>
+    <t>6 months or less</t>
+  </si>
+  <si>
+    <t>more_than_6_months</t>
+  </si>
+  <si>
+    <t>More than 6 months</t>
+  </si>
+  <si>
+    <t>all_life</t>
+  </si>
+  <si>
+    <t>All life</t>
+  </si>
+  <si>
+    <t>xr9ir97</t>
+  </si>
+  <si>
+    <t>jw3gq75</t>
+  </si>
+  <si>
+    <t>full_time</t>
+  </si>
+  <si>
+    <t>Full-time</t>
+  </si>
+  <si>
+    <t>part_time</t>
+  </si>
+  <si>
+    <t>Part-time</t>
+  </si>
+  <si>
+    <t>wd0pj17</t>
+  </si>
+  <si>
+    <t>sales_or_service</t>
+  </si>
+  <si>
+    <t>Sales or service</t>
+  </si>
+  <si>
+    <t>clerical_or_administrative_support</t>
+  </si>
+  <si>
+    <t>Clerical or administrative support</t>
+  </si>
+  <si>
+    <t>manufacturing__construction__maintenance</t>
+  </si>
+  <si>
+    <t>Manufacturing, construction, maintenance, or farming</t>
+  </si>
+  <si>
+    <t>professional__managerial__or_technical</t>
+  </si>
+  <si>
+    <t>Professional, managerial, or technical</t>
+  </si>
+  <si>
+    <t>bj9uk70</t>
+  </si>
+  <si>
+    <t>zd25i60</t>
+  </si>
+  <si>
+    <t>xp5yr96</t>
+  </si>
+  <si>
+    <t>mn8kr20</t>
+  </si>
+  <si>
+    <t>monday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>tuesday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>wednesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>thursday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>friday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>saturday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>sunday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
   </si>
   <si>
     <t>style</t>
@@ -650,7 +1067,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,15 +1145,21 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -751,57 +1174,54 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -814,13 +1234,30 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -830,15 +1267,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -846,357 +1283,1684 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" t="s">
+        <v>149</v>
+      </c>
+      <c r="D62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>151</v>
+      </c>
+      <c r="B65" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>151</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>164</v>
+      </c>
+      <c r="B75" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>164</v>
+      </c>
+      <c r="B76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>164</v>
+      </c>
+      <c r="B77" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" t="s">
+        <v>67</v>
+      </c>
+      <c r="C79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>170</v>
+      </c>
+      <c r="B81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" t="s">
+        <v>129</v>
+      </c>
+      <c r="D81" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>170</v>
+      </c>
+      <c r="B82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" t="s">
+        <v>133</v>
+      </c>
+      <c r="D83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" t="s">
+        <v>150</v>
+      </c>
+      <c r="D84" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" t="s">
+        <v>173</v>
+      </c>
+      <c r="D85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" t="s">
+        <v>68</v>
+      </c>
+      <c r="D86" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" t="s">
+        <v>171</v>
+      </c>
+      <c r="C87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>129</v>
+      </c>
+      <c r="C88" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>174</v>
+      </c>
+      <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" t="s">
+        <v>150</v>
+      </c>
+      <c r="C91" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>174</v>
+      </c>
+      <c r="B92" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93" t="s">
+        <v>67</v>
+      </c>
+      <c r="C93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>175</v>
+      </c>
+      <c r="B94" t="s">
+        <v>171</v>
+      </c>
+      <c r="C94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>175</v>
+      </c>
+      <c r="B96" t="s">
+        <v>132</v>
+      </c>
+      <c r="C96" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" t="s">
+        <v>133</v>
+      </c>
+      <c r="C97" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" t="s">
+        <v>176</v>
+      </c>
+      <c r="C98" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>175</v>
+      </c>
+      <c r="B99" t="s">
+        <v>67</v>
+      </c>
+      <c r="C99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>178</v>
+      </c>
+      <c r="B100" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" t="s">
+        <v>181</v>
+      </c>
+      <c r="C101" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>178</v>
+      </c>
+      <c r="B102" t="s">
+        <v>183</v>
+      </c>
+      <c r="C102" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" t="s">
+        <v>185</v>
+      </c>
+      <c r="C103" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>178</v>
+      </c>
+      <c r="B104" t="s">
+        <v>187</v>
+      </c>
+      <c r="C104" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>178</v>
+      </c>
+      <c r="B105" t="s">
+        <v>189</v>
+      </c>
+      <c r="C105" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>178</v>
+      </c>
+      <c r="B106" t="s">
+        <v>191</v>
+      </c>
+      <c r="C106" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" t="s">
+        <v>67</v>
+      </c>
+      <c r="C107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>193</v>
+      </c>
+      <c r="B108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C108" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>193</v>
+      </c>
+      <c r="B109" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110" t="s">
+        <v>67</v>
+      </c>
+      <c r="C110" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>194</v>
+      </c>
+      <c r="B111" t="s">
+        <v>195</v>
+      </c>
+      <c r="C111" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>194</v>
+      </c>
+      <c r="B112" t="s">
+        <v>197</v>
+      </c>
+      <c r="C112" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>194</v>
+      </c>
+      <c r="B113" t="s">
+        <v>199</v>
+      </c>
+      <c r="C113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>194</v>
+      </c>
+      <c r="B114" t="s">
+        <v>67</v>
+      </c>
+      <c r="C114" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>201</v>
+      </c>
+      <c r="B115" t="s">
+        <v>79</v>
+      </c>
+      <c r="C115" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>201</v>
+      </c>
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>201</v>
+      </c>
+      <c r="B117" t="s">
+        <v>67</v>
+      </c>
+      <c r="C117" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>202</v>
+      </c>
+      <c r="B118" t="s">
+        <v>203</v>
+      </c>
+      <c r="C118" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>202</v>
+      </c>
+      <c r="B119" t="s">
+        <v>205</v>
+      </c>
+      <c r="C119" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>202</v>
+      </c>
+      <c r="B120" t="s">
+        <v>67</v>
+      </c>
+      <c r="C120" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>207</v>
+      </c>
+      <c r="B121" t="s">
+        <v>208</v>
+      </c>
+      <c r="C121" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>207</v>
+      </c>
+      <c r="B122" t="s">
+        <v>210</v>
+      </c>
+      <c r="C122" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>207</v>
+      </c>
+      <c r="B123" t="s">
+        <v>212</v>
+      </c>
+      <c r="C123" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>207</v>
+      </c>
+      <c r="B124" t="s">
+        <v>214</v>
+      </c>
+      <c r="C124" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>207</v>
+      </c>
+      <c r="B125" t="s">
+        <v>76</v>
+      </c>
+      <c r="C125" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>207</v>
+      </c>
+      <c r="B126" t="s">
+        <v>67</v>
+      </c>
+      <c r="C126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>216</v>
+      </c>
+      <c r="B127" t="s">
+        <v>79</v>
+      </c>
+      <c r="C127" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>216</v>
+      </c>
+      <c r="B128" t="s">
+        <v>81</v>
+      </c>
+      <c r="C128" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>216</v>
+      </c>
+      <c r="B129" t="s">
+        <v>67</v>
+      </c>
+      <c r="C129" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>217</v>
+      </c>
+      <c r="B130" t="s">
+        <v>79</v>
+      </c>
+      <c r="C130" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>217</v>
+      </c>
+      <c r="B131" t="s">
+        <v>81</v>
+      </c>
+      <c r="C131" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>217</v>
+      </c>
+      <c r="B132" t="s">
+        <v>67</v>
+      </c>
+      <c r="C132" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>218</v>
+      </c>
+      <c r="B133" t="s">
+        <v>171</v>
+      </c>
+      <c r="C133" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>218</v>
+      </c>
+      <c r="B134" t="s">
+        <v>129</v>
+      </c>
+      <c r="C134" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>218</v>
+      </c>
+      <c r="B135" t="s">
+        <v>132</v>
+      </c>
+      <c r="C135" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>218</v>
+      </c>
+      <c r="B136" t="s">
+        <v>133</v>
+      </c>
+      <c r="C136" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>218</v>
+      </c>
+      <c r="B137" t="s">
+        <v>150</v>
+      </c>
+      <c r="C137" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>218</v>
+      </c>
+      <c r="B138" t="s">
+        <v>165</v>
+      </c>
+      <c r="C138" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>218</v>
+      </c>
+      <c r="B139" t="s">
+        <v>166</v>
+      </c>
+      <c r="C139" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>218</v>
+      </c>
+      <c r="B140" t="s">
+        <v>167</v>
+      </c>
+      <c r="C140" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>218</v>
+      </c>
+      <c r="B141" t="s">
+        <v>67</v>
+      </c>
+      <c r="C141" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>219</v>
+      </c>
+      <c r="B142" t="s">
+        <v>220</v>
+      </c>
+      <c r="C142" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>219</v>
+      </c>
+      <c r="B143" t="s">
+        <v>222</v>
+      </c>
+      <c r="C143" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>219</v>
+      </c>
+      <c r="B144" t="s">
+        <v>224</v>
+      </c>
+      <c r="C144" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>219</v>
+      </c>
+      <c r="B145" t="s">
+        <v>226</v>
+      </c>
+      <c r="C145" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>219</v>
+      </c>
+      <c r="B146" t="s">
+        <v>228</v>
+      </c>
+      <c r="C146" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>219</v>
+      </c>
+      <c r="B147" t="s">
+        <v>230</v>
+      </c>
+      <c r="C147" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>219</v>
+      </c>
+      <c r="B148" t="s">
+        <v>232</v>
+      </c>
+      <c r="C148" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>219</v>
+      </c>
+      <c r="B149" t="s">
+        <v>67</v>
+      </c>
+      <c r="C149" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1214,24 +2978,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>